<commit_message>
Bulk Entry With Excel File
</commit_message>
<xml_diff>
--- a/ITL_MakeId.Web/wwwroot/Uploads/Book1.xlsx
+++ b/ITL_MakeId.Web/wwwroot/Uploads/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF204577-6D4A-4867-B3D3-74DCEACFCE5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{464D5F74-5965-4DD9-BA40-25E9348FC80A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4CA015C0-2237-46E5-9F33-2022645C22B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B0EE828A-5AE9-4DF4-9406-CC2BB86CBB7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Id</t>
   </si>
@@ -33,64 +33,58 @@
     <t>Name</t>
   </si>
   <si>
+    <t>DesignationId</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>BloodGroupId</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>ImagePathOfUser</t>
+  </si>
+  <si>
+    <t>ImagePathOfUserSignature</t>
+  </si>
+  <si>
+    <t>ImagePathOfAuthorizedSignature</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>CompanyAddress</t>
+  </si>
+  <si>
+    <t>CompanyLogoPath</t>
+  </si>
+  <si>
+    <t>CardInfo</t>
+  </si>
+  <si>
+    <t>ValidationStartDate</t>
+  </si>
+  <si>
+    <t>ValidationEndDate</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>IssueDate</t>
+  </si>
+  <si>
+    <t>CardCategoryId</t>
+  </si>
+  <si>
     <t>Hasan</t>
   </si>
   <si>
-    <t>Tamal</t>
-  </si>
-  <si>
-    <t>DesignationId</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>BloodGroupId</t>
-  </si>
-  <si>
-    <t>CardNumber</t>
-  </si>
-  <si>
-    <t>ImagePathOfUser</t>
-  </si>
-  <si>
-    <t>ImagePathOfUserSignature</t>
-  </si>
-  <si>
-    <t>ImagePathOfAuthorizedSignature</t>
-  </si>
-  <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>CompanyAddress</t>
-  </si>
-  <si>
-    <t>CompanyLogoPath</t>
-  </si>
-  <si>
-    <t>CardInfo</t>
-  </si>
-  <si>
-    <t>ValidationStartDate</t>
-  </si>
-  <si>
-    <t>ValidationEndDate</t>
-  </si>
-  <si>
-    <t>DateOfBirth</t>
-  </si>
-  <si>
-    <t>IssueDate</t>
-  </si>
-  <si>
-    <t>CardCategoryId</t>
-  </si>
-  <si>
-    <t>ITL-0001</t>
-  </si>
-  <si>
-    <t>a9dcb966-b4f1-4dce-8579-2b0711a340b7_saiful-bin-a-kalam-passport-size-photo.jpg</t>
+    <t>ITL-0005</t>
   </si>
   <si>
     <t>NULL</t>
@@ -103,34 +97,14 @@
   </si>
   <si>
     <t>This card should be used by card holder only. If this card is found ownerless, please, returnit to the issuing authority. This card is not transferable to anybody.</t>
-  </si>
-  <si>
-    <t>0001-01-01 00:00:00.0000000</t>
-  </si>
-  <si>
-    <t>ITL-0002</t>
-  </si>
-  <si>
-    <t>ITL-0003</t>
-  </si>
-  <si>
-    <t>ITL-0004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -158,10 +132,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,97 +447,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFB150F-1E7E-4E00-9C1A-B98004A01B17}">
-  <dimension ref="A1:R5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB34AE80-0BB7-4F37-BA89-8C2F0B9CF870}">
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="54" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="143.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -577,191 +529,40 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="2">
-        <v>44068</v>
-      </c>
-      <c r="O2" s="2">
-        <v>44079</v>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
       </c>
       <c r="P2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="Q2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>